<commit_message>
stock , data driven
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Dec 05, 2023, 20:04</t>
   </si>
   <si>
-    <t xml:space="preserve">entecavir monohydrate 50 microgram/mL oral liquid</t>
+    <t xml:space="preserve">Soflax (AN) tablet</t>
   </si>
   <si>
     <t xml:space="preserve">Drug safe retrieval</t>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dec 05, 2023, 17:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soflax (AN) tablet</t>
   </si>
   <si>
     <t xml:space="preserve">Adjustment</t>
@@ -227,11 +224,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -247,6 +245,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -291,8 +294,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,10 +323,10 @@
   <dimension ref="B1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.57"/>
   </cols>
@@ -353,11 +360,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -474,13 +481,13 @@
         <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>21</v>
@@ -503,13 +510,13 @@
         <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>21</v>
@@ -521,7 +528,7 @@
         <v>14</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>14</v>
@@ -529,236 +536,236 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="D14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="D16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="G16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="0" t="s">
+      <c r="I16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="D26" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="D28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data driven madication , and qty from xlsx file = stocktake
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -64,33 +64,36 @@
     <t xml:space="preserve">sam rigers</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 05, 2023, 17:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norspan 20 microgram/hour patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receipt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aut cumque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arvind Nath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Person</t>
+  </si>
+  <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 05, 2023, 17:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norspan 20 microgram/hour patch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Receipt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aut cumque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arvind Nath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Person</t>
-  </si>
-  <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
@@ -146,9 +149,6 @@
   </si>
   <si>
     <t xml:space="preserve">101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">35</t>
@@ -224,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -245,11 +245,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,7 +294,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,10 +318,10 @@
   <dimension ref="B1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.57"/>
   </cols>
@@ -412,18 +407,18 @@
         <v>15</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>19</v>
@@ -438,21 +433,21 @@
         <v>22</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>19</v>
@@ -467,27 +462,27 @@
         <v>22</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>21</v>
@@ -496,27 +491,27 @@
         <v>22</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>21</v>
@@ -525,62 +520,62 @@
         <v>22</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>43</v>
@@ -594,19 +589,19 @@
         <v>45</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>46</v>
@@ -620,19 +615,19 @@
         <v>48</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J20" s="0" t="s">
         <v>49</v>
@@ -646,19 +641,19 @@
         <v>51</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J22" s="0" t="s">
         <v>52</v>
@@ -672,19 +667,19 @@
         <v>54</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>55</v>
@@ -698,19 +693,19 @@
         <v>57</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J26" s="0" t="s">
         <v>58</v>
@@ -724,19 +719,19 @@
         <v>60</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J28" s="0" t="s">
         <v>61</v>
@@ -750,19 +745,19 @@
         <v>63</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J30" s="0" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Stocktake = datadriven , Medication name , qty = done
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -52,103 +52,103 @@
     <t xml:space="preserve">Dec 05, 2023, 20:04</t>
   </si>
   <si>
+    <t xml:space="preserve">amoxicillin 500 mg capsule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug safe retrieval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nancy Holt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sam rigers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 05, 2023, 17:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norspan 20 microgram/hour patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receipt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aut cumque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arvind Nath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 05, 2023, 17:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzemet 100 mg/5 mL injection, 5 mL ampoule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 05, 2023, 17:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avastin 400 mg/16 mL injection, 16 mL vial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 05, 2023, 17:02</t>
+  </si>
+  <si>
     <t xml:space="preserve">Soflax (AN) tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">Drug safe retrieval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nancy Holt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sam rigers</t>
+    <t xml:space="preserve">Adjustment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endone XR 40 mg modified release tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 05, 2023, 00:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zinc oxide 15.25% cream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wing 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 04, 2023, 22:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 05, 2023, 17:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norspan 20 microgram/hour patch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Receipt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aut cumque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arvind Nath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 05, 2023, 17:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anzemet 100 mg/5 mL injection, 5 mL ampoule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 05, 2023, 17:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avastin 400 mg/16 mL injection, 16 mL vial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 05, 2023, 17:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adjustment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endone XR 40 mg modified release tablet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 05, 2023, 00:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zinc oxide 15.25% cream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transfer in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wing 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 04, 2023, 22:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amoxicillin 500 mg capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101</t>
   </si>
   <si>
     <t xml:space="preserve">35</t>
@@ -289,12 +289,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,10 +314,10 @@
   <dimension ref="B1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.57"/>
   </cols>
@@ -359,7 +355,7 @@
       <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -410,15 +406,15 @@
         <v>23</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>19</v>
@@ -433,21 +429,21 @@
         <v>22</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>19</v>
@@ -462,21 +458,21 @@
         <v>22</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>31</v>
@@ -491,18 +487,18 @@
         <v>22</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>33</v>
@@ -560,19 +556,19 @@
         <v>40</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="G16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>23</v>
@@ -592,13 +588,13 @@
         <v>37</v>
       </c>
       <c r="E18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>23</v>
@@ -618,13 +614,13 @@
         <v>37</v>
       </c>
       <c r="E20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>23</v>
@@ -644,13 +640,13 @@
         <v>37</v>
       </c>
       <c r="E22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>23</v>
@@ -670,13 +666,13 @@
         <v>37</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>23</v>
@@ -696,13 +692,13 @@
         <v>37</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>23</v>
@@ -722,13 +718,13 @@
         <v>37</v>
       </c>
       <c r="E28" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>23</v>
@@ -748,13 +744,13 @@
         <v>37</v>
       </c>
       <c r="E30" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
stock sheet = trasferin multipule times with same medication name
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -311,18 +311,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:J30"/>
+  <dimension ref="B1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
@@ -380,12 +380,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>19</v>
@@ -400,27 +429,56 @@
         <v>22</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>21</v>
@@ -435,128 +493,252 @@
         <v>23</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>23</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>37</v>
@@ -574,188 +756,6 @@
         <v>23</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="0" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Balance = dynamic drug name , dynamic qty pass from sheet Opening balance and Closing balance written into sheet
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">11</t>
@@ -286,13 +283,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -315,10 +316,13 @@
   <dimension ref="B1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.84"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -368,266 +372,266 @@
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>15</v>
+      <c r="I7" s="2" t="n">
+        <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>15</v>
+      <c r="J8" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>15</v>
+      <c r="I9" s="2" t="n">
+        <v>8</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
@@ -640,89 +644,89 @@
       <c r="H12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>15</v>
+      <c r="I12" s="2" t="n">
+        <v>9</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="H15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>15</v>
+      <c r="I15" s="2" t="n">
+        <v>3</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>14</v>
@@ -730,11 +734,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
@@ -747,11 +751,11 @@
       <c r="H16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>15</v>
+      <c r="I16" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balance = Working fine taking all drug name and qty from sheet
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -64,48 +64,30 @@
     <t xml:space="preserve">Test Person</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 07, 2023, 15:48</t>
   </si>
   <si>
     <t xml:space="preserve">amoxicillin 500 mg capsule</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 07, 2023, 15:46</t>
   </si>
   <si>
     <t xml:space="preserve">bromocriptine 5 mg capsule</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 07, 2023, 15:28</t>
   </si>
   <si>
     <t xml:space="preserve">clotrimazole 1% lotion</t>
   </si>
   <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 07, 2023, 15:24</t>
   </si>
   <si>
     <t xml:space="preserve">doxazosin 4 mg tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 07, 2023, 14:53</t>
   </si>
   <si>
@@ -121,9 +103,6 @@
     <t xml:space="preserve">Lisa Lawson</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
     <t xml:space="preserve">everolimus 10 mg tablet</t>
   </si>
   <si>
@@ -142,9 +121,6 @@
     <t xml:space="preserve">John Demo</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 07, 2023, 14:06</t>
   </si>
   <si>
@@ -154,18 +130,12 @@
     <t xml:space="preserve">Drug safe retrieval</t>
   </si>
   <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 06, 2023, 22:24</t>
   </si>
   <si>
     <t xml:space="preserve">wool fat 1 g/g ointment</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 06, 2023, 22:23</t>
   </si>
   <si>
@@ -178,16 +148,10 @@
     <t xml:space="preserve">lidocaine hydrochloride 4% cream</t>
   </si>
   <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dec 06, 2023, 22:03</t>
   </si>
   <si>
     <t xml:space="preserve">methadone hydrochloride 500 microgram/mL oral liquid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">Dec 06, 2023, 22:02</t>
@@ -283,13 +247,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -316,12 +284,19 @@
   <dimension ref="B1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,22 +344,18 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="H2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -395,22 +366,18 @@
       <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="H3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -421,22 +388,18 @@
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="H4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -447,22 +410,18 @@
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="H5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -473,138 +432,118 @@
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="H6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="H7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="2" t="n">
+      <c r="H9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -615,22 +554,18 @@
       <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="H11" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -641,22 +576,18 @@
       <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="H12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -667,22 +598,18 @@
       <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="H13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -693,51 +620,43 @@
       <c r="G14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="H14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="I15" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
@@ -748,15 +667,11 @@
       <c r="G16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="H16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Balance fixed : Medication name
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -239,13 +239,13 @@
   <dimension ref="B1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>

</xml_diff>

<commit_message>
Balance : Location selection dynamic
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t xml:space="preserve">Date (Static)</t>
   </si>
@@ -55,79 +55,73 @@
     <t xml:space="preserve">Transfer in</t>
   </si>
   <si>
-    <t xml:space="preserve">101</t>
+    <t xml:space="preserve">WA Nursing Home</t>
   </si>
   <si>
     <t xml:space="preserve">(amoxicillin) amoxicillin 500 mg capsule</t>
   </si>
   <si>
+    <t xml:space="preserve">External facility</t>
+  </si>
+  <si>
     <t xml:space="preserve">(bromocriptine) bromocriptine 5 mg capsule</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">(clotrimazole) clotrimazole 1% lotion</t>
   </si>
   <si>
+    <t xml:space="preserve">Wing A</t>
+  </si>
+  <si>
     <t xml:space="preserve">(doxazosin) doxazosin 4 mg tablet</t>
   </si>
   <si>
     <t xml:space="preserve">(buprenorphine) Norspan 20 microgram/hour patch</t>
   </si>
   <si>
-    <t xml:space="preserve">102</t>
+    <t xml:space="preserve">sub loc 2</t>
   </si>
   <si>
     <t xml:space="preserve">(everolimus) everolimus 10 mg tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">103</t>
+    <t xml:space="preserve">Integration Level 1</t>
   </si>
   <si>
     <t xml:space="preserve">(fluorouracil) fluorouracil 5% cream</t>
   </si>
   <si>
-    <t xml:space="preserve">104</t>
+    <t xml:space="preserve">Integration level 1</t>
   </si>
   <si>
     <t xml:space="preserve">(oxycodone) Endone 5 mg tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">105</t>
+    <t xml:space="preserve">Room 5</t>
   </si>
   <si>
     <t xml:space="preserve">(wool fat) wool fat 1 g/g ointment</t>
   </si>
   <si>
-    <t xml:space="preserve">106</t>
-  </si>
-  <si>
     <t xml:space="preserve">(gentamicin) gentamicin 40 mg/mL injection, ampoule</t>
   </si>
   <si>
-    <t xml:space="preserve">107</t>
-  </si>
-  <si>
     <t xml:space="preserve">(lidocaine) lidocaine hydrochloride 4% cream</t>
   </si>
   <si>
-    <t xml:space="preserve">108</t>
-  </si>
-  <si>
     <t xml:space="preserve">(methadone) methadone hydrochloride 500 microgram/mL oral liquid</t>
   </si>
   <si>
-    <t xml:space="preserve">109</t>
-  </si>
-  <si>
     <t xml:space="preserve">(prilocaine) prilocaine hydrochloride 1% (50 mg/5 mL) injection, ampoule</t>
   </si>
   <si>
-    <t xml:space="preserve">110</t>
-  </si>
-  <si>
     <t xml:space="preserve">(amoxicillin) Yomax 500 mg capsule</t>
   </si>
   <si>
-    <t xml:space="preserve">111</t>
+    <t xml:space="preserve">sub loc 1</t>
   </si>
 </sst>
 </file>
@@ -212,11 +206,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -236,13 +230,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:J16"/>
+  <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
@@ -291,14 +285,14 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,198 +303,198 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="I11" s="3"/>
+      <c r="H11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="2" t="n">
+      <c r="H12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>29</v>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,52 +505,61 @@
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>31</v>
+      <c r="E14" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>33</v>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>35</v>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="2" t="n">
+      <c r="H16" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="I16" s="3"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
TestNG : BalanceTest , xml
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t xml:space="preserve">Date (Static)</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Action (Static)</t>
   </si>
   <si>
-    <t xml:space="preserve">To/From (Static)</t>
+    <t xml:space="preserve">To/From (Location)</t>
   </si>
   <si>
     <t xml:space="preserve">Resident (Static)</t>
@@ -61,46 +61,40 @@
     <t xml:space="preserve">(amoxicillin) amoxicillin 500 mg capsule</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(bromocriptine) bromocriptine 5 mg capsule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(clotrimazole) clotrimazole 1% lotion</t>
+  </si>
+  <si>
     <t xml:space="preserve">External facility</t>
   </si>
   <si>
-    <t xml:space="preserve">(bromocriptine) bromocriptine 5 mg capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(clotrimazole) clotrimazole 1% lotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wing A</t>
-  </si>
-  <si>
     <t xml:space="preserve">(doxazosin) doxazosin 4 mg tablet</t>
   </si>
   <si>
     <t xml:space="preserve">(buprenorphine) Norspan 20 microgram/hour patch</t>
   </si>
   <si>
-    <t xml:space="preserve">sub loc 2</t>
+    <t xml:space="preserve">Pharmacy</t>
   </si>
   <si>
     <t xml:space="preserve">(everolimus) everolimus 10 mg tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">Integration Level 1</t>
+    <t xml:space="preserve">Internal Facility 2</t>
   </si>
   <si>
     <t xml:space="preserve">(fluorouracil) fluorouracil 5% cream</t>
   </si>
   <si>
-    <t xml:space="preserve">Integration level 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">(oxycodone) Endone 5 mg tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">Room 5</t>
+    <t xml:space="preserve">Final Facility</t>
   </si>
   <si>
     <t xml:space="preserve">(wool fat) wool fat 1 g/g ointment</t>
@@ -115,13 +109,19 @@
     <t xml:space="preserve">(methadone) methadone hydrochloride 500 microgram/mL oral liquid</t>
   </si>
   <si>
+    <t xml:space="preserve">Imprest</t>
+  </si>
+  <si>
     <t xml:space="preserve">(prilocaine) prilocaine hydrochloride 1% (50 mg/5 mL) injection, ampoule</t>
   </si>
   <si>
+    <t xml:space="preserve">Loc-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">(amoxicillin) Yomax 500 mg capsule</t>
   </si>
   <si>
-    <t xml:space="preserve">sub loc 1</t>
+    <t xml:space="preserve">overall ecase</t>
   </si>
 </sst>
 </file>
@@ -236,12 +236,12 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.45"/>
@@ -321,8 +321,8 @@
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
+      <c r="E4" s="2" t="n">
+        <v>101</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="3" t="n">
@@ -334,13 +334,13 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="3" t="n">
@@ -352,13 +352,13 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
+      <c r="E6" s="2" t="n">
+        <v>102</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="3" t="n">
@@ -370,13 +370,13 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -389,13 +389,13 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -408,13 +408,13 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>24</v>
+      <c r="E9" s="2" t="n">
+        <v>6</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -427,13 +427,13 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -446,13 +446,13 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
+      <c r="E11" s="2" t="n">
+        <v>105</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="n">
@@ -464,13 +464,13 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
+      <c r="E12" s="2" t="n">
+        <v>103</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="3" t="n">
@@ -482,13 +482,13 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>15</v>
+      <c r="E13" s="2" t="n">
+        <v>104</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3" t="n">
@@ -500,13 +500,13 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="3" t="n">
@@ -518,13 +518,13 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>

</xml_diff>

<commit_message>
TestNG : BalanceTest : testng.xml : working fine
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -233,19 +233,17 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="1.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Page object model TestNG , Stock Balance TestNG
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Table Data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -233,10 +234,10 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
@@ -568,4 +569,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Page object model sheet working = drug , location , QTY
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t xml:space="preserve">Date (Static)</t>
   </si>
@@ -68,34 +68,34 @@
     <t xml:space="preserve">(bromocriptine) bromocriptine 5 mg capsule</t>
   </si>
   <si>
+    <t xml:space="preserve">External facility</t>
+  </si>
+  <si>
     <t xml:space="preserve">(clotrimazole) clotrimazole 1% lotion</t>
   </si>
   <si>
-    <t xml:space="preserve">External facility</t>
+    <t xml:space="preserve">Final Facility</t>
   </si>
   <si>
     <t xml:space="preserve">(doxazosin) doxazosin 4 mg tablet</t>
   </si>
   <si>
+    <t xml:space="preserve">Pharmacy</t>
+  </si>
+  <si>
     <t xml:space="preserve">(buprenorphine) Norspan 20 microgram/hour patch</t>
   </si>
   <si>
-    <t xml:space="preserve">Pharmacy</t>
+    <t xml:space="preserve">Internal Facility 2</t>
   </si>
   <si>
     <t xml:space="preserve">(everolimus) everolimus 10 mg tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">Internal Facility 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">(fluorouracil) fluorouracil 5% cream</t>
   </si>
   <si>
     <t xml:space="preserve">(oxycodone) Endone 5 mg tablet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final Facility</t>
   </si>
   <si>
     <t xml:space="preserve">(wool fat) wool fat 1 g/g ointment</t>
@@ -234,10 +234,10 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
@@ -320,8 +320,8 @@
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>101</v>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="3" t="n">
@@ -333,13 +333,13 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="3" t="n">
@@ -351,13 +351,13 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>102</v>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="3" t="n">
@@ -369,13 +369,13 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -388,7 +388,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
@@ -407,7 +407,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
@@ -426,13 +426,13 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -486,8 +486,8 @@
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>104</v>
+      <c r="E13" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3" t="n">
@@ -582,7 +582,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
TestNG = POM = Login Dynamic
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t xml:space="preserve">Date (Static)</t>
   </si>
@@ -123,6 +123,30 @@
   </si>
   <si>
     <t xml:space="preserve">overall ecase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username/email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strongroompassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Facility - West Ward</t>
   </si>
 </sst>
 </file>
@@ -233,11 +257,11 @@
   </sheetPr>
   <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
@@ -576,14 +600,49 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Transfer in patient = TestNG = POM
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t xml:space="preserve">Date (Static)</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">To/From (Location)</t>
   </si>
   <si>
-    <t xml:space="preserve">Resident (Static)</t>
+    <t xml:space="preserve">Resident</t>
   </si>
   <si>
     <t xml:space="preserve">Entered By (Static)</t>
@@ -59,60 +59,96 @@
     <t xml:space="preserve">WA Nursing Home</t>
   </si>
   <si>
+    <t xml:space="preserve">Arvind Nath</t>
+  </si>
+  <si>
     <t xml:space="preserve">(amoxicillin) amoxicillin 500 mg capsule</t>
   </si>
   <si>
     <t xml:space="preserve">Facility 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Windsor Charles</t>
+  </si>
+  <si>
     <t xml:space="preserve">(bromocriptine) bromocriptine 5 mg capsule</t>
   </si>
   <si>
     <t xml:space="preserve">External facility</t>
   </si>
   <si>
+    <t xml:space="preserve">Wilbur Smith</t>
+  </si>
+  <si>
     <t xml:space="preserve">(clotrimazole) clotrimazole 1% lotion</t>
   </si>
   <si>
     <t xml:space="preserve">Final Facility</t>
   </si>
   <si>
+    <t xml:space="preserve">Jerry RAC004</t>
+  </si>
+  <si>
     <t xml:space="preserve">(doxazosin) doxazosin 4 mg tablet</t>
   </si>
   <si>
     <t xml:space="preserve">Pharmacy</t>
   </si>
   <si>
+    <t xml:space="preserve">Ita Rooney</t>
+  </si>
+  <si>
     <t xml:space="preserve">(buprenorphine) Norspan 20 microgram/hour patch</t>
   </si>
   <si>
     <t xml:space="preserve">Internal Facility 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Robyn Dhar</t>
+  </si>
+  <si>
     <t xml:space="preserve">(everolimus) everolimus 10 mg tablet</t>
   </si>
   <si>
+    <t xml:space="preserve">Robert Jones</t>
+  </si>
+  <si>
     <t xml:space="preserve">(fluorouracil) fluorouracil 5% cream</t>
   </si>
   <si>
+    <t xml:space="preserve">Ted Bryan</t>
+  </si>
+  <si>
     <t xml:space="preserve">(oxycodone) Endone 5 mg tablet</t>
   </si>
   <si>
     <t xml:space="preserve">(wool fat) wool fat 1 g/g ointment</t>
   </si>
   <si>
+    <t xml:space="preserve">Michael ILU</t>
+  </si>
+  <si>
     <t xml:space="preserve">(gentamicin) gentamicin 40 mg/mL injection, ampoule</t>
   </si>
   <si>
+    <t xml:space="preserve">Pamela Butler</t>
+  </si>
+  <si>
     <t xml:space="preserve">(lidocaine) lidocaine hydrochloride 4% cream</t>
   </si>
   <si>
+    <t xml:space="preserve">Perry Grant</t>
+  </si>
+  <si>
     <t xml:space="preserve">(methadone) methadone hydrochloride 500 microgram/mL oral liquid</t>
   </si>
   <si>
     <t xml:space="preserve">Imprest</t>
   </si>
   <si>
+    <t xml:space="preserve">David Springer</t>
+  </si>
+  <si>
     <t xml:space="preserve">(prilocaine) prilocaine hydrochloride 1% (50 mg/5 mL) injection, ampoule</t>
   </si>
   <si>
@@ -123,6 +159,9 @@
   </si>
   <si>
     <t xml:space="preserve">overall ecase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matilda Kerr</t>
   </si>
   <si>
     <t xml:space="preserve">Location</t>
@@ -156,7 +195,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -177,6 +216,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,6 +280,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -257,17 +305,18 @@
   </sheetPr>
   <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="1.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.42"/>
   </cols>
   <sheetData>
@@ -311,6 +360,9 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="3" t="n">
         <v>1</v>
@@ -321,13 +373,16 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="n">
@@ -339,13 +394,16 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="3" t="n">
@@ -357,13 +415,16 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="3" t="n">
@@ -375,13 +436,16 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="3" t="n">
@@ -393,15 +457,17 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="3" t="n">
         <v>6</v>
@@ -412,15 +478,17 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="3" t="n">
         <v>7</v>
@@ -431,15 +499,17 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="3" t="n">
         <v>8</v>
@@ -450,15 +520,17 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="3" t="n">
         <v>9</v>
@@ -469,13 +541,16 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="n">
@@ -487,13 +562,16 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="3" t="n">
@@ -505,13 +583,16 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3" t="n">
@@ -523,13 +604,16 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="3" t="n">
@@ -541,15 +625,17 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="3" t="n">
         <v>14</v>
@@ -560,13 +646,16 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="3" t="n">
@@ -602,11 +691,11 @@
   </sheetPr>
   <dimension ref="B1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.14"/>
@@ -616,30 +705,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestNG = POM = Adjustment in progress
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -21,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
-  <si>
-    <t xml:space="preserve">Date (Static)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+  <si>
+    <t xml:space="preserve">Transection ID</t>
   </si>
   <si>
     <t xml:space="preserve">Drug</t>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">Balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5e26790f-e97b-47a9-978b-e42b5915acbc</t>
   </si>
   <si>
     <t xml:space="preserve">(docusate + sennoside B) Soflax (AN) tablet</t>
@@ -195,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -216,11 +219,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -265,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,10 +278,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -306,12 +300,13 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
@@ -350,18 +345,20 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="3" t="n">
@@ -373,16 +370,16 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="n">
@@ -394,16 +391,16 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="3" t="n">
@@ -415,16 +412,16 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="3" t="n">
@@ -436,16 +433,16 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="3" t="n">
@@ -457,16 +454,16 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="3" t="n">
@@ -478,16 +475,16 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="3" t="n">
@@ -499,16 +496,16 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="3" t="n">
@@ -520,16 +517,16 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="3" t="n">
@@ -541,16 +538,16 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="n">
@@ -562,16 +559,16 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="3" t="n">
@@ -583,16 +580,16 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>38</v>
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3" t="n">
@@ -604,16 +601,16 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="3" t="n">
@@ -625,16 +622,16 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="3" t="n">
@@ -646,16 +643,16 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="3" t="n">
@@ -695,7 +692,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.14"/>
@@ -705,30 +702,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>